<commit_message>
Expand units to monetary values
The tool previously supported monetary quantities in a very superficial fashion.  Monetary quantities are now supported as well throughout as emissions, production, and other quantities have been for some time.

This required making some adjustments to input files, test cases, documentation, etc.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/DataProviderTemplate.xlsx
+++ b/docs/DataProviderTemplate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/MichaelTiemannOSC/ITR/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_BCCFA2BD0AFE4771E24C6D0DBC87A6ED4B30D22F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35A3BBCA-F2EF-46A8-B156-4D9ACA454480}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4455F6B-D6AA-8A4D-9299-68DBDB6D7FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="target_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>company_name</t>
   </si>
@@ -199,13 +199,19 @@
   </si>
   <si>
     <t>Steel</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +223,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,9 +286,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:Q51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R51" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:R51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="isic"/>
@@ -289,6 +301,7 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="sector"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ghg_s1s2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ghg_s3"/>
+    <tableColumn id="14" xr3:uid="{6DCBAC65-5237-9448-A67A-5749F6FFEAEB}" name="currency"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="company_revenue"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="company_market_cap"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="company_enterprise_value"/>
@@ -587,26 +600,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,22 +657,25 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -696,23 +712,26 @@
       <c r="L2">
         <v>61888133</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2">
         <v>7370536918</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>7318942238</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>24392175674</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>21337139</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>990719858</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -749,23 +768,27 @@
       <c r="L3">
         <v>18413448.829999998</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3">
         <v>2795781568</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3615211346</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>3620291185</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>43581896.049999997</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>463981837.19999999</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -778,25 +801,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="4" width="21.140625" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="4" width="21.1640625" customWidth="1"/>
+    <col min="6" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +869,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -887,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -932,7 +955,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1161,6 +1184,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1169,20 +1198,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>